<commit_message>
Wohnmobil instead of Wohnwagen
</commit_message>
<xml_diff>
--- a/data/BFS/raw/BFS_Fahrzeugbestand_CH.xlsx
+++ b/data/BFS/raw/BFS_Fahrzeugbestand_CH.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="DieseArbeitsmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/research/RGithubLearning/Bernd_Autos/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/admin/research/RGithubLearning/Bernd_Autos/data/BFS/raw/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEBA9807-31BE-414C-97BC-7CB7173E54B5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC6D151-F620-9D4C-864B-19246E99903B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="720" windowWidth="25600" windowHeight="15080" tabRatio="782" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="720" windowWidth="25600" windowHeight="15080" tabRatio="782" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2019" sheetId="39" r:id="rId1"/>
@@ -2698,9 +2698,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+    <sheetView zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <selection pane="bottomLeft" activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -3966,9 +3966,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:K61"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="A39" sqref="A39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -24350,7 +24350,7 @@
   <dimension ref="A1:L59"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
+      <pane ySplit="9" topLeftCell="A12" activePane="bottomLeft" state="frozenSplit"/>
       <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -34507,7 +34507,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A1:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -51988,7 +51988,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="9" topLeftCell="A10" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomLeft" activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.5" defaultRowHeight="11" x14ac:dyDescent="0.15"/>
@@ -52091,7 +52091,7 @@
       <c r="J6" s="11"/>
       <c r="K6" s="28"/>
     </row>
-    <row r="7" spans="1:11" ht="3.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="7" spans="1:11" ht="30" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="8" spans="1:11" ht="12.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="16" t="s">
         <v>24</v>

</xml_diff>